<commit_message>
update floyd-warshall with scipy and from daniel
</commit_message>
<xml_diff>
--- a/from daniel/test.xlsx
+++ b/from daniel/test.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Downloads\from daniel\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Thesis - Algorithm\from daniel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1B9A930F-7FBE-48AF-830C-08D7851DF2A9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{51E552F5-2529-4CD1-9351-E0ABB8337EBA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="15840" xr2:uid="{7874F2F7-1779-4AF4-BE2E-C06D7F36DB9A}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="15840" activeTab="2" xr2:uid="{7874F2F7-1779-4AF4-BE2E-C06D7F36DB9A}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -18,6 +18,7 @@
     <sheet name="7matrix" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
+  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -526,7 +527,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7F8B1CFD-843B-4606-8686-D8B95D8359D6}">
   <dimension ref="A1:Q278"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
@@ -2112,12 +2113,14 @@
   <dimension ref="A1:Y25"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="K9" sqref="K9"/>
+      <selection activeCell="E1" sqref="E1:E1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="25" width="5.7109375" style="6" customWidth="1"/>
+    <col min="2" max="2" width="5.7109375" style="6" customWidth="1"/>
+    <col min="3" max="5" width="10" style="6" bestFit="1" customWidth="1"/>
+    <col min="6" max="25" width="5.7109375" style="6" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:25" x14ac:dyDescent="0.25">
@@ -2304,11 +2307,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9D95A216-4019-41AF-AF46-F7B553D0C99C}">
   <dimension ref="A1:H8"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G10" sqref="G10"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="M14" sqref="M14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="4" bestFit="1" customWidth="1"/>
+    <col min="2" max="7" width="10" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="7.28515625" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B1" t="s">

</xml_diff>